<commit_message>
BL creation beta ready in docs section ready
</commit_message>
<xml_diff>
--- a/templates/BL.xlsx
+++ b/templates/BL.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Desktop\Projects\tsAddin\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC2F5B8B-8ACB-4947-9446-5F21418878CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B0BBE3D-0E6F-4694-B7CE-8C3F55FC7EDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3270" yWindow="2573" windowWidth="21600" windowHeight="11482" xr2:uid="{BF1809CB-C232-4AA5-B44F-479B0C20AC5C}"/>
+    <workbookView xWindow="1470" yWindow="1470" windowWidth="21600" windowHeight="11580" xr2:uid="{BF1809CB-C232-4AA5-B44F-479B0C20AC5C}"/>
   </bookViews>
   <sheets>
     <sheet name="BL" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="13">
   <si>
     <t>Shipper</t>
   </si>
@@ -92,9 +92,6 @@
   </si>
   <si>
     <t xml:space="preserve"> PCS / Quantity</t>
-  </si>
-  <si>
-    <t>Сорт</t>
   </si>
 </sst>
 </file>
@@ -727,7 +724,7 @@
   <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -816,7 +813,7 @@
       </c>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" ht="26.65" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="7" t="s">
         <v>1</v>
       </c>
@@ -887,7 +884,7 @@
         <v>1</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="D14" s="24" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
group by same bl added
</commit_message>
<xml_diff>
--- a/templates/BL.xlsx
+++ b/templates/BL.xlsx
@@ -8,29 +8,29 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B0BBE3D-0E6F-4694-B7CE-8C3F55FC7EDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{297C4228-1A8C-4CDE-AF38-C5523FC3AEBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="1470" windowWidth="21600" windowHeight="11580" xr2:uid="{BF1809CB-C232-4AA5-B44F-479B0C20AC5C}"/>
+    <workbookView xWindow="-55778" yWindow="-98" windowWidth="28995" windowHeight="15796" xr2:uid="{BF1809CB-C232-4AA5-B44F-479B0C20AC5C}"/>
   </bookViews>
   <sheets>
     <sheet name="BL" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="Bl">BL!$A$14</definedName>
-    <definedName name="Всего">BL!$F$14</definedName>
-    <definedName name="Дата">BL!$A$8</definedName>
-    <definedName name="Куда">BL!$A$10</definedName>
-    <definedName name="Места">BL!$E$14</definedName>
-    <definedName name="Откуда">BL!$B$10</definedName>
-    <definedName name="Получатель">BL!$A$5</definedName>
-    <definedName name="Получатель_адрес">BL!$A$6</definedName>
-    <definedName name="Продавец">BL!$A$2</definedName>
-    <definedName name="Продавец_адрес">BL!$A$3</definedName>
-    <definedName name="Продукт">BL!$B$14</definedName>
-    <definedName name="Сорт">BL!$C$14</definedName>
-    <definedName name="Судно">BL!$B$8</definedName>
-    <definedName name="Транспорт">BL!$C$8</definedName>
-    <definedName name="Упаковка">BL!$D$14</definedName>
+    <definedName name="Bl_массив">BL!$B$14</definedName>
+    <definedName name="Всего">BL!$G$14</definedName>
+    <definedName name="Дата">BL!$B$8</definedName>
+    <definedName name="Куда">BL!$B$10</definedName>
+    <definedName name="Места">BL!$F$14</definedName>
+    <definedName name="Откуда">BL!$C$10</definedName>
+    <definedName name="Получатель">BL!$B$5</definedName>
+    <definedName name="Получатель_адрес">BL!$B$6</definedName>
+    <definedName name="Продавец">BL!$B$2</definedName>
+    <definedName name="Продавец_адрес">BL!$B$3</definedName>
+    <definedName name="Продукт">BL!$C$14</definedName>
+    <definedName name="Сорт">BL!$D$14</definedName>
+    <definedName name="Судно">BL!$C$8</definedName>
+    <definedName name="Транспорт">BL!$D$8</definedName>
+    <definedName name="Упаковка">BL!$E$14</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -293,7 +293,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -301,23 +301,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -364,6 +349,24 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -721,290 +724,345 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E29E8F5-D6CC-40FA-A28F-FB98CEB6F079}">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" customWidth="1"/>
-    <col min="2" max="2" width="31.33203125" customWidth="1"/>
-    <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="4" width="11" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" customWidth="1"/>
-    <col min="6" max="6" width="16.33203125" customWidth="1"/>
-    <col min="7" max="7" width="18.796875" customWidth="1"/>
-    <col min="8" max="8" width="18.33203125" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" customWidth="1"/>
-    <col min="10" max="10" width="9.1328125" customWidth="1"/>
-    <col min="11" max="11" width="56" customWidth="1"/>
-    <col min="12" max="12" width="12.33203125" customWidth="1"/>
-    <col min="13" max="13" width="10.33203125" customWidth="1"/>
-    <col min="14" max="17" width="9.1328125" customWidth="1"/>
-    <col min="18" max="18" width="9.796875" customWidth="1"/>
-    <col min="19" max="20" width="9.1328125" customWidth="1"/>
-    <col min="21" max="21" width="11.796875" customWidth="1"/>
-    <col min="22" max="23" width="9.1328125" customWidth="1"/>
-    <col min="24" max="24" width="13.1328125" customWidth="1"/>
-    <col min="25" max="27" width="9.1328125" customWidth="1"/>
+    <col min="1" max="1" width="1.86328125" customWidth="1"/>
+    <col min="2" max="2" width="14.19921875" customWidth="1"/>
+    <col min="3" max="3" width="40.59765625" customWidth="1"/>
+    <col min="4" max="4" width="16.3984375" customWidth="1"/>
+    <col min="5" max="5" width="11" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" customWidth="1"/>
+    <col min="8" max="8" width="1.3984375" customWidth="1"/>
+    <col min="9" max="9" width="18.33203125" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" customWidth="1"/>
+    <col min="11" max="11" width="9.1328125" customWidth="1"/>
+    <col min="12" max="12" width="56" customWidth="1"/>
+    <col min="13" max="13" width="12.33203125" customWidth="1"/>
+    <col min="14" max="14" width="10.33203125" customWidth="1"/>
+    <col min="15" max="18" width="9.1328125" customWidth="1"/>
+    <col min="19" max="19" width="9.796875" customWidth="1"/>
+    <col min="20" max="21" width="9.1328125" customWidth="1"/>
+    <col min="22" max="22" width="11.796875" customWidth="1"/>
+    <col min="23" max="24" width="9.1328125" customWidth="1"/>
+    <col min="25" max="25" width="13.1328125" customWidth="1"/>
+    <col min="26" max="28" width="9.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A1" s="33" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A1" s="3"/>
+      <c r="B1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34"/>
       <c r="C1" s="35"/>
-      <c r="D1" s="1"/>
+      <c r="D1" s="36"/>
       <c r="E1" s="1"/>
-      <c r="F1" s="2"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A2" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="37"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="11"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A2" s="3"/>
+      <c r="B2" s="37" t="s">
+        <v>1</v>
+      </c>
       <c r="C2" s="38"/>
-      <c r="F2" s="3"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A3" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="37"/>
+      <c r="D2" s="39"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="11"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A3" s="3"/>
+      <c r="B3" s="37" t="s">
+        <v>1</v>
+      </c>
       <c r="C3" s="38"/>
-      <c r="F3" s="3"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A4" s="33" t="s">
+      <c r="D3" s="39"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="11"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A4" s="3"/>
+      <c r="B4" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="34"/>
       <c r="C4" s="35"/>
-      <c r="F4" s="3"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A5" s="39" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="40"/>
+      <c r="D4" s="36"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="11"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A5" s="3"/>
+      <c r="B5" s="40" t="s">
+        <v>1</v>
+      </c>
       <c r="C5" s="41"/>
-      <c r="F5" s="3"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A6" s="42" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="43"/>
+      <c r="D5" s="42"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="11"/>
+    </row>
+    <row r="6" spans="1:8" ht="25.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="3"/>
+      <c r="B6" s="43" t="s">
+        <v>1</v>
+      </c>
       <c r="C6" s="44"/>
-      <c r="F6" s="3"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A7" s="4" t="s">
+      <c r="D6" s="45"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="11"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A7" s="3"/>
+      <c r="B7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="C7" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="D7" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="3"/>
-    </row>
-    <row r="8" spans="1:6" ht="26.65" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="F8" s="3"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A9" s="10" t="s">
+      <c r="G7" s="3"/>
+      <c r="H7" s="11"/>
+    </row>
+    <row r="8" spans="1:8" ht="26.65" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="3"/>
+      <c r="B8" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="G8" s="3"/>
+      <c r="H8" s="11"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A9" s="3"/>
+      <c r="B9" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="C9" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="12"/>
-      <c r="F9" s="3"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A10" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" s="15"/>
-      <c r="F10" s="3"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A11" s="16"/>
-      <c r="C11" s="17"/>
-      <c r="F11" s="3"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A12" s="18"/>
-      <c r="B12" s="19"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="15"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A13" s="21" t="s">
+      <c r="D9" s="7"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="11"/>
+    </row>
+    <row r="10" spans="1:8" ht="25.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="3"/>
+      <c r="B10" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="10"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="11"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A11" s="3"/>
+      <c r="B11" s="11"/>
+      <c r="D11" s="12"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="11"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A12" s="3"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="11"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A13" s="3"/>
+      <c r="B13" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="22" t="s">
+      <c r="C13" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="23" t="s">
+      <c r="D13" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="22" t="s">
+      <c r="E13" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="31" t="s">
+      <c r="F13" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="F13" s="32"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A14" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B14" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="D14" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="E14" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="F14" s="26" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A15" s="27"/>
-      <c r="B15" s="28"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="30"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A16" s="7"/>
-      <c r="B16" s="24"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="26"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A17" s="7"/>
-      <c r="B17" s="24"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="26"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A18" s="7"/>
-      <c r="B18" s="24"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="26"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A19" s="7"/>
-      <c r="B19" s="24"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="26"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A20" s="7"/>
-      <c r="B20" s="24"/>
-      <c r="C20" s="24"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="24"/>
-      <c r="F20" s="26"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A21" s="7"/>
-      <c r="B21" s="24"/>
-      <c r="C21" s="24"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="24"/>
-      <c r="F21" s="26"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A22" s="7"/>
-      <c r="B22" s="24"/>
-      <c r="C22" s="24"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="26"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A23" s="7"/>
-      <c r="B23" s="24"/>
-      <c r="C23" s="24"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="24"/>
-      <c r="F23" s="26"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A24" s="7"/>
-      <c r="B24" s="24"/>
-      <c r="C24" s="24"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="24"/>
-      <c r="F24" s="26"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A25" s="7"/>
-      <c r="B25" s="24"/>
-      <c r="C25" s="24"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="24"/>
-      <c r="F25" s="26"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A26" s="16"/>
-      <c r="F26" s="3"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A27" s="18"/>
-      <c r="B27" s="19"/>
-      <c r="C27" s="19"/>
-      <c r="D27" s="19"/>
-      <c r="E27" s="19"/>
-      <c r="F27" s="15"/>
+      <c r="G13" s="33"/>
+      <c r="H13" s="11"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A14" s="3"/>
+      <c r="B14" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="F14" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="G14" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="H14" s="11"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A15" s="3"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="11"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A16" s="3"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="21"/>
+      <c r="H16" s="11"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A17" s="3"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="11"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A18" s="3"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="11"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A19" s="3"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="11"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A20" s="3"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="11"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A21" s="3"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="11"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A22" s="3"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="11"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A23" s="3"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="21"/>
+      <c r="H23" s="11"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A24" s="3"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="11"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A25" s="3"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="11"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A26" s="3"/>
+      <c r="B26" s="11"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="11"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A27" s="3"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:D6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
height bug in excel template fixed, init rows functions generalized
</commit_message>
<xml_diff>
--- a/templates/BL.xlsx
+++ b/templates/BL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{297C4228-1A8C-4CDE-AF38-C5523FC3AEBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A73BDBEE-5A79-4C18-B7E6-A751339C03B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-55778" yWindow="-98" windowWidth="28995" windowHeight="15796" xr2:uid="{BF1809CB-C232-4AA5-B44F-479B0C20AC5C}"/>
+    <workbookView xWindow="-26978" yWindow="-98" windowWidth="27076" windowHeight="16395" xr2:uid="{BF1809CB-C232-4AA5-B44F-479B0C20AC5C}"/>
   </bookViews>
   <sheets>
     <sheet name="BL" sheetId="1" r:id="rId1"/>
@@ -98,17 +98,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -155,6 +146,23 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -298,117 +306,117 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -727,7 +735,7 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -757,11 +765,11 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" s="3"/>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="35"/>
-      <c r="D1" s="36"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="31"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="2"/>
@@ -769,51 +777,51 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" s="3"/>
-      <c r="B2" s="37" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="39"/>
+      <c r="B2" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="33"/>
+      <c r="D2" s="34"/>
       <c r="G2" s="3"/>
       <c r="H2" s="11"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="3"/>
-      <c r="B3" s="37" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="39"/>
+      <c r="B3" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="33"/>
+      <c r="D3" s="34"/>
       <c r="G3" s="3"/>
       <c r="H3" s="11"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" s="3"/>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="35"/>
-      <c r="D4" s="36"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="31"/>
       <c r="G4" s="3"/>
       <c r="H4" s="11"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="3"/>
-      <c r="B5" s="40" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="41"/>
-      <c r="D5" s="42"/>
+      <c r="B5" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="36"/>
+      <c r="D5" s="37"/>
       <c r="G5" s="3"/>
       <c r="H5" s="11"/>
     </row>
     <row r="6" spans="1:8" ht="25.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="3"/>
-      <c r="B6" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="44"/>
-      <c r="D6" s="45"/>
+      <c r="B6" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="39"/>
+      <c r="D6" s="40"/>
       <c r="G6" s="3"/>
       <c r="H6" s="11"/>
     </row>
@@ -822,10 +830,10 @@
       <c r="B7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="28" t="s">
+      <c r="C7" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="30" t="s">
+      <c r="D7" s="27" t="s">
         <v>5</v>
       </c>
       <c r="G7" s="3"/>
@@ -833,13 +841,13 @@
     </row>
     <row r="8" spans="1:8" ht="26.65" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="3"/>
-      <c r="B8" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="29" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" s="31" t="s">
+      <c r="B8" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="28" t="s">
         <v>1</v>
       </c>
       <c r="G8" s="3"/>
@@ -847,7 +855,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9" s="3"/>
-      <c r="B9" s="27" t="s">
+      <c r="B9" s="24" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="6" t="s">
@@ -888,22 +896,22 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A13" s="3"/>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="18" t="s">
+      <c r="D13" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="17" t="s">
+      <c r="E13" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="F13" s="32" t="s">
+      <c r="F13" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="G13" s="33"/>
+      <c r="G13" s="45"/>
       <c r="H13" s="11"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.45">
@@ -911,131 +919,131 @@
       <c r="B14" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="D14" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="E14" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="F14" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="G14" s="21" t="s">
+      <c r="C14" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="F14" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="G14" s="18" t="s">
         <v>1</v>
       </c>
       <c r="H14" s="11"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15" s="3"/>
-      <c r="B15" s="22"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="25"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="22"/>
       <c r="H15" s="11"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A16" s="3"/>
       <c r="B16" s="5"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="21"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="18"/>
       <c r="H16" s="11"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A17" s="3"/>
       <c r="B17" s="5"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="21"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="18"/>
       <c r="H17" s="11"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A18" s="3"/>
       <c r="B18" s="5"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="21"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="18"/>
       <c r="H18" s="11"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A19" s="3"/>
       <c r="B19" s="5"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="21"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="18"/>
       <c r="H19" s="11"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A20" s="3"/>
       <c r="B20" s="5"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="21"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="18"/>
       <c r="H20" s="11"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A21" s="3"/>
       <c r="B21" s="5"/>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="21"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="18"/>
       <c r="H21" s="11"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A22" s="3"/>
       <c r="B22" s="5"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="21"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="18"/>
       <c r="H22" s="11"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A23" s="3"/>
       <c r="B23" s="5"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="21"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="18"/>
       <c r="H23" s="11"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A24" s="3"/>
       <c r="B24" s="5"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="21"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="18"/>
       <c r="H24" s="11"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A25" s="3"/>
       <c r="B25" s="5"/>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="21"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="18"/>
       <c r="H25" s="11"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
beta bl gross added to tmp + spPack added
</commit_message>
<xml_diff>
--- a/templates/BL.xlsx
+++ b/templates/BL.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A73BDBEE-5A79-4C18-B7E6-A751339C03B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E71BA61-5305-4AF8-8160-6B8925E01027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-26978" yWindow="-98" windowWidth="27076" windowHeight="16395" xr2:uid="{BF1809CB-C232-4AA5-B44F-479B0C20AC5C}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <definedNames>
     <definedName name="Bl_массив">BL!$B$14</definedName>
-    <definedName name="Всего">BL!$G$14</definedName>
+    <definedName name="Всего">BL!$H$14</definedName>
     <definedName name="Дата">BL!$B$8</definedName>
     <definedName name="Куда">BL!$B$10</definedName>
     <definedName name="Места">BL!$F$14</definedName>
@@ -33,6 +33,7 @@
     <definedName name="Упаковка">BL!$E$14</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -53,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
   <si>
     <t>Shipper</t>
   </si>
@@ -91,7 +92,13 @@
     <t>Kind of pkgs</t>
   </si>
   <si>
-    <t xml:space="preserve"> PCS / Quantity</t>
+    <t>Unit count</t>
+  </si>
+  <si>
+    <t>Net weight</t>
+  </si>
+  <si>
+    <t>Gross weight</t>
   </si>
 </sst>
 </file>
@@ -301,7 +308,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -367,6 +374,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -402,21 +421,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -730,12 +734,30 @@
 </a:theme>
 </file>
 
+<file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
+<wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
+  <wetp:taskpane dockstate="right" visibility="0" width="700" row="2">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </wetp:taskpane>
+</wetp:taskpanes>
+</file>
+
+<file path=xl/webextensions/webextension1.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{6C7422AA-0A6B-4D88-A02C-632F9DFF40E9}">
+  <we:reference id="5dbca137-d02b-4283-adec-e6f28aeb3ed7" version="1.0.0.0" store="developer" storeType="Registry"/>
+  <we:alternateReferences/>
+  <we:properties/>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</we:webextension>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E29E8F5-D6CC-40FA-A28F-FB98CEB6F079}">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -745,87 +767,88 @@
     <col min="3" max="3" width="40.59765625" customWidth="1"/>
     <col min="4" max="4" width="16.3984375" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" customWidth="1"/>
-    <col min="7" max="7" width="16.33203125" customWidth="1"/>
-    <col min="8" max="8" width="1.3984375" customWidth="1"/>
-    <col min="9" max="9" width="18.33203125" customWidth="1"/>
-    <col min="10" max="10" width="11.6640625" customWidth="1"/>
-    <col min="11" max="11" width="9.1328125" customWidth="1"/>
-    <col min="12" max="12" width="56" customWidth="1"/>
-    <col min="13" max="13" width="12.33203125" customWidth="1"/>
-    <col min="14" max="14" width="10.33203125" customWidth="1"/>
-    <col min="15" max="18" width="9.1328125" customWidth="1"/>
-    <col min="19" max="19" width="9.796875" customWidth="1"/>
-    <col min="20" max="21" width="9.1328125" customWidth="1"/>
-    <col min="22" max="22" width="11.796875" customWidth="1"/>
-    <col min="23" max="24" width="9.1328125" customWidth="1"/>
-    <col min="25" max="25" width="13.1328125" customWidth="1"/>
-    <col min="26" max="28" width="9.1328125" customWidth="1"/>
+    <col min="6" max="7" width="14.33203125" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" customWidth="1"/>
+    <col min="9" max="9" width="1.3984375" customWidth="1"/>
+    <col min="10" max="10" width="18.33203125" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" customWidth="1"/>
+    <col min="12" max="12" width="9.1328125" customWidth="1"/>
+    <col min="13" max="13" width="56" customWidth="1"/>
+    <col min="14" max="14" width="12.33203125" customWidth="1"/>
+    <col min="15" max="15" width="10.33203125" customWidth="1"/>
+    <col min="16" max="19" width="9.1328125" customWidth="1"/>
+    <col min="20" max="20" width="9.796875" customWidth="1"/>
+    <col min="21" max="22" width="9.1328125" customWidth="1"/>
+    <col min="23" max="23" width="11.796875" customWidth="1"/>
+    <col min="24" max="25" width="9.1328125" customWidth="1"/>
+    <col min="26" max="26" width="13.1328125" customWidth="1"/>
+    <col min="27" max="29" width="9.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" s="3"/>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="31"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="35"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="11"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G1" s="1"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="11"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" s="3"/>
-      <c r="B2" s="32" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="34"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="11"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B2" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="37"/>
+      <c r="D2" s="38"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="11"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="3"/>
-      <c r="B3" s="32" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="33"/>
-      <c r="D3" s="34"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="11"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B3" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="37"/>
+      <c r="D3" s="38"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="11"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="3"/>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="30"/>
-      <c r="D4" s="31"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="11"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="C4" s="34"/>
+      <c r="D4" s="35"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="11"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="3"/>
-      <c r="B5" s="35" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="36"/>
-      <c r="D5" s="37"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="11"/>
-    </row>
-    <row r="6" spans="1:8" ht="25.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B5" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="40"/>
+      <c r="D5" s="41"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="11"/>
+    </row>
+    <row r="6" spans="1:9" ht="25.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="3"/>
-      <c r="B6" s="38" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="39"/>
-      <c r="D6" s="40"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="11"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B6" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="43"/>
+      <c r="D6" s="44"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="11"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" s="3"/>
       <c r="B7" s="4" t="s">
         <v>3</v>
@@ -836,10 +859,10 @@
       <c r="D7" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="3"/>
-      <c r="H7" s="11"/>
-    </row>
-    <row r="8" spans="1:8" ht="26.65" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="H7" s="3"/>
+      <c r="I7" s="11"/>
+    </row>
+    <row r="8" spans="1:9" ht="26.65" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="3"/>
       <c r="B8" s="23" t="s">
         <v>1</v>
@@ -850,10 +873,10 @@
       <c r="D8" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="G8" s="3"/>
-      <c r="H8" s="11"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="H8" s="3"/>
+      <c r="I8" s="11"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" s="3"/>
       <c r="B9" s="24" t="s">
         <v>6</v>
@@ -862,10 +885,10 @@
         <v>7</v>
       </c>
       <c r="D9" s="7"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="11"/>
-    </row>
-    <row r="10" spans="1:8" ht="25.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="H9" s="3"/>
+      <c r="I9" s="11"/>
+    </row>
+    <row r="10" spans="1:9" ht="25.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="3"/>
       <c r="B10" s="8" t="s">
         <v>1</v>
@@ -874,47 +897,53 @@
         <v>1</v>
       </c>
       <c r="D10" s="10"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="11"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="H10" s="3"/>
+      <c r="I10" s="11"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" s="3"/>
       <c r="B11" s="11"/>
       <c r="D11" s="12"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="11"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="H11" s="3"/>
+      <c r="I11" s="11"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" s="3"/>
       <c r="B12" s="13"/>
       <c r="C12" s="14"/>
       <c r="D12" s="15"/>
       <c r="E12" s="14"/>
       <c r="F12" s="14"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="11"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G12" s="14"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="11"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" s="3"/>
-      <c r="B13" s="41" t="s">
+      <c r="B13" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="42" t="s">
+      <c r="C13" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="43" t="s">
+      <c r="D13" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="42" t="s">
+      <c r="E13" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="F13" s="44" t="s">
+      <c r="F13" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="G13" s="45"/>
-      <c r="H13" s="11"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G13" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="I13" s="11"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" s="3"/>
       <c r="B14" s="5" t="s">
         <v>1</v>
@@ -931,146 +960,160 @@
       <c r="F14" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="G14" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="H14" s="11"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G14" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="H14" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="I14" s="11"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" s="3"/>
       <c r="B15" s="19"/>
       <c r="C15" s="20"/>
       <c r="D15" s="17"/>
       <c r="E15" s="21"/>
       <c r="F15" s="21"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="11"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G15" s="21"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="11"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" s="3"/>
       <c r="B16" s="5"/>
       <c r="C16" s="16"/>
       <c r="D16" s="16"/>
       <c r="E16" s="16"/>
       <c r="F16" s="16"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="11"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G16" s="16"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="11"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" s="3"/>
       <c r="B17" s="5"/>
       <c r="C17" s="16"/>
       <c r="D17" s="16"/>
       <c r="E17" s="16"/>
       <c r="F17" s="16"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="11"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G17" s="16"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="11"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18" s="3"/>
       <c r="B18" s="5"/>
       <c r="C18" s="16"/>
       <c r="D18" s="16"/>
       <c r="E18" s="16"/>
       <c r="F18" s="16"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="11"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G18" s="16"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="11"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" s="3"/>
       <c r="B19" s="5"/>
       <c r="C19" s="16"/>
       <c r="D19" s="16"/>
       <c r="E19" s="16"/>
       <c r="F19" s="16"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="11"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G19" s="16"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="11"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20" s="3"/>
       <c r="B20" s="5"/>
       <c r="C20" s="16"/>
       <c r="D20" s="16"/>
       <c r="E20" s="16"/>
       <c r="F20" s="16"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="11"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G20" s="16"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="11"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21" s="3"/>
       <c r="B21" s="5"/>
       <c r="C21" s="16"/>
       <c r="D21" s="16"/>
       <c r="E21" s="16"/>
       <c r="F21" s="16"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="11"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G21" s="16"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="11"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A22" s="3"/>
       <c r="B22" s="5"/>
       <c r="C22" s="16"/>
       <c r="D22" s="16"/>
       <c r="E22" s="16"/>
       <c r="F22" s="16"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="11"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G22" s="16"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="11"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23" s="3"/>
       <c r="B23" s="5"/>
       <c r="C23" s="16"/>
       <c r="D23" s="16"/>
       <c r="E23" s="16"/>
       <c r="F23" s="16"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="11"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G23" s="16"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="11"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24" s="3"/>
       <c r="B24" s="5"/>
       <c r="C24" s="16"/>
       <c r="D24" s="16"/>
       <c r="E24" s="16"/>
       <c r="F24" s="16"/>
-      <c r="G24" s="18"/>
-      <c r="H24" s="11"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G24" s="16"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="11"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A25" s="3"/>
       <c r="B25" s="5"/>
       <c r="C25" s="16"/>
       <c r="D25" s="16"/>
       <c r="E25" s="16"/>
       <c r="F25" s="16"/>
-      <c r="G25" s="18"/>
-      <c r="H25" s="11"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G25" s="16"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="11"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A26" s="3"/>
       <c r="B26" s="11"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="11"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="H26" s="3"/>
+      <c r="I26" s="11"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A27" s="3"/>
       <c r="B27" s="13"/>
       <c r="C27" s="14"/>
       <c r="D27" s="14"/>
       <c r="E27" s="14"/>
       <c r="F27" s="14"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="11"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="F13:G13"/>
+  <mergeCells count="6">
+    <mergeCell ref="B6:D6"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B6:D6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
reice no fixed port letter tmp, work on new bl tmp started
</commit_message>
<xml_diff>
--- a/templates/BL.xlsx
+++ b/templates/BL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E71BA61-5305-4AF8-8160-6B8925E01027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47F9CCD4-7894-4F59-9506-954FC7217304}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26978" yWindow="-98" windowWidth="27076" windowHeight="16395" xr2:uid="{BF1809CB-C232-4AA5-B44F-479B0C20AC5C}"/>
+    <workbookView xWindow="4170" yWindow="6165" windowWidth="13425" windowHeight="8385" xr2:uid="{BF1809CB-C232-4AA5-B44F-479B0C20AC5C}"/>
   </bookViews>
   <sheets>
     <sheet name="BL" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,6 @@
     <definedName name="Упаковка">BL!$E$14</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -386,6 +385,15 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -411,15 +419,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -440,9 +439,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -480,7 +479,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -586,7 +585,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -728,7 +727,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -757,7 +756,7 @@
   <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="B6" sqref="B6:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -787,11 +786,11 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" s="3"/>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="35"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="38"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -800,51 +799,51 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" s="3"/>
-      <c r="B2" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="38"/>
+      <c r="B2" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="40"/>
+      <c r="D2" s="41"/>
       <c r="H2" s="3"/>
       <c r="I2" s="11"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="3"/>
-      <c r="B3" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="37"/>
-      <c r="D3" s="38"/>
+      <c r="B3" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="40"/>
+      <c r="D3" s="41"/>
       <c r="H3" s="3"/>
       <c r="I3" s="11"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="3"/>
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="34"/>
-      <c r="D4" s="35"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="38"/>
       <c r="H4" s="3"/>
       <c r="I4" s="11"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="3"/>
-      <c r="B5" s="39" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="40"/>
-      <c r="D5" s="41"/>
+      <c r="B5" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="43"/>
+      <c r="D5" s="44"/>
       <c r="H5" s="3"/>
       <c r="I5" s="11"/>
     </row>
     <row r="6" spans="1:9" ht="25.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="3"/>
-      <c r="B6" s="42" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="43"/>
-      <c r="D6" s="44"/>
+      <c r="B6" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="34"/>
+      <c r="D6" s="35"/>
       <c r="H6" s="3"/>
       <c r="I6" s="11"/>
     </row>

</xml_diff>

<commit_message>
bl measure mts replased on kg
</commit_message>
<xml_diff>
--- a/templates/BL.xlsx
+++ b/templates/BL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7F5D6BB-8C9F-4031-869A-F51C155EC458}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F095979-2E9E-4041-BF3B-AE541B1BE505}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28702" yWindow="83" windowWidth="27076" windowHeight="16995" tabRatio="667" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="27076" windowHeight="16395" tabRatio="667" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BL" sheetId="10" r:id="rId1"/>
@@ -669,9 +669,39 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -692,36 +722,6 @@
     </xf>
     <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1004,8 +1004,8 @@
   </sheetPr>
   <dimension ref="A1:N69"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6" defaultRowHeight="10.15"/>
@@ -1018,7 +1018,7 @@
     <col min="6" max="6" width="7.375" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.4375" style="3" customWidth="1"/>
     <col min="8" max="8" width="13.75" style="3" customWidth="1"/>
-    <col min="9" max="9" width="12.0625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="13.875" style="3" customWidth="1"/>
     <col min="10" max="10" width="8.75" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6" style="2"/>
     <col min="12" max="12" width="7.375" style="2" bestFit="1" customWidth="1"/>
@@ -1033,58 +1033,58 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="12" customHeight="1">
-      <c r="A2" s="92" t="s">
+      <c r="A2" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="92"/>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="92"/>
+      <c r="B2" s="77"/>
+      <c r="C2" s="77"/>
+      <c r="D2" s="77"/>
+      <c r="E2" s="77"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="4"/>
     </row>
     <row r="3" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A3" s="87" t="s">
+      <c r="A3" s="78" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="87"/>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="93" t="s">
+      <c r="B3" s="78"/>
+      <c r="C3" s="78"/>
+      <c r="D3" s="78"/>
+      <c r="E3" s="78"/>
+      <c r="F3" s="79" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="93"/>
-      <c r="H3" s="93"/>
+      <c r="G3" s="79"/>
+      <c r="H3" s="79"/>
       <c r="I3" s="2" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="13.5" customHeight="1">
-      <c r="A4" s="88" t="s">
+      <c r="A4" s="80" t="s">
         <v>51</v>
       </c>
-      <c r="B4" s="88"/>
-      <c r="C4" s="88"/>
-      <c r="D4" s="88"/>
-      <c r="E4" s="88"/>
-      <c r="F4" s="94" t="s">
+      <c r="B4" s="80"/>
+      <c r="C4" s="80"/>
+      <c r="D4" s="80"/>
+      <c r="E4" s="80"/>
+      <c r="F4" s="81" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="94"/>
-      <c r="H4" s="94"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="81"/>
       <c r="I4" s="6"/>
     </row>
     <row r="5" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A5" s="88" t="s">
+      <c r="A5" s="80" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="88"/>
-      <c r="C5" s="88"/>
-      <c r="D5" s="88"/>
-      <c r="E5" s="88"/>
+      <c r="B5" s="80"/>
+      <c r="C5" s="80"/>
+      <c r="D5" s="80"/>
+      <c r="E5" s="80"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
       <c r="H5" s="7" t="s">
@@ -1093,82 +1093,82 @@
       <c r="I5" s="7"/>
     </row>
     <row r="6" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A6" s="90"/>
-      <c r="B6" s="90"/>
-      <c r="C6" s="90"/>
-      <c r="D6" s="90"/>
-      <c r="E6" s="90"/>
+      <c r="A6" s="82"/>
+      <c r="B6" s="82"/>
+      <c r="C6" s="82"/>
+      <c r="D6" s="82"/>
+      <c r="E6" s="82"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
     </row>
     <row r="7" spans="1:12" ht="12" customHeight="1">
-      <c r="A7" s="87" t="s">
+      <c r="A7" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="87"/>
-      <c r="C7" s="87"/>
-      <c r="D7" s="87"/>
-      <c r="E7" s="87"/>
+      <c r="B7" s="78"/>
+      <c r="C7" s="78"/>
+      <c r="D7" s="78"/>
+      <c r="E7" s="78"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
     </row>
     <row r="8" spans="1:12" ht="12" customHeight="1">
-      <c r="A8" s="91" t="s">
+      <c r="A8" s="83" t="s">
         <v>66</v>
       </c>
-      <c r="B8" s="91"/>
-      <c r="C8" s="91"/>
-      <c r="D8" s="91"/>
-      <c r="E8" s="91"/>
+      <c r="B8" s="83"/>
+      <c r="C8" s="83"/>
+      <c r="D8" s="83"/>
+      <c r="E8" s="83"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
     </row>
     <row r="9" spans="1:12" ht="15.4" customHeight="1">
-      <c r="A9" s="88" t="s">
+      <c r="A9" s="80" t="s">
         <v>65</v>
       </c>
-      <c r="B9" s="88"/>
-      <c r="C9" s="88"/>
-      <c r="D9" s="88"/>
-      <c r="E9" s="88"/>
+      <c r="B9" s="80"/>
+      <c r="C9" s="80"/>
+      <c r="D9" s="80"/>
+      <c r="E9" s="80"/>
       <c r="I9" s="6"/>
     </row>
     <row r="10" spans="1:12" ht="15.4" customHeight="1">
-      <c r="A10" s="88"/>
-      <c r="B10" s="88"/>
-      <c r="C10" s="88"/>
-      <c r="D10" s="88"/>
-      <c r="E10" s="88"/>
+      <c r="A10" s="80"/>
+      <c r="B10" s="80"/>
+      <c r="C10" s="80"/>
+      <c r="D10" s="80"/>
+      <c r="E10" s="80"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
     </row>
     <row r="11" spans="1:12" ht="15.4" customHeight="1">
-      <c r="A11" s="88"/>
-      <c r="B11" s="88"/>
-      <c r="C11" s="88"/>
-      <c r="D11" s="88"/>
-      <c r="E11" s="88"/>
+      <c r="A11" s="80"/>
+      <c r="B11" s="80"/>
+      <c r="C11" s="80"/>
+      <c r="D11" s="80"/>
+      <c r="E11" s="80"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
     </row>
     <row r="12" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A12" s="87" t="s">
+      <c r="A12" s="78" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="87"/>
-      <c r="C12" s="87"/>
-      <c r="D12" s="87"/>
-      <c r="E12" s="87"/>
+      <c r="B12" s="78"/>
+      <c r="C12" s="78"/>
+      <c r="D12" s="78"/>
+      <c r="E12" s="78"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
@@ -1188,24 +1188,24 @@
       <c r="I13" s="69"/>
     </row>
     <row r="14" spans="1:12" ht="15.4" customHeight="1">
-      <c r="A14" s="88" t="s">
+      <c r="A14" s="80" t="s">
         <v>68</v>
       </c>
-      <c r="B14" s="88"/>
-      <c r="C14" s="88"/>
-      <c r="D14" s="88"/>
-      <c r="E14" s="88"/>
+      <c r="B14" s="80"/>
+      <c r="C14" s="80"/>
+      <c r="D14" s="80"/>
+      <c r="E14" s="80"/>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
     </row>
     <row r="15" spans="1:12" ht="15.4" customHeight="1">
-      <c r="A15" s="88"/>
-      <c r="B15" s="88"/>
-      <c r="C15" s="88"/>
-      <c r="D15" s="88"/>
-      <c r="E15" s="88"/>
+      <c r="A15" s="80"/>
+      <c r="B15" s="80"/>
+      <c r="C15" s="80"/>
+      <c r="D15" s="80"/>
+      <c r="E15" s="80"/>
       <c r="F15" s="7"/>
       <c r="G15" s="7" t="s">
         <v>5</v>
@@ -1215,11 +1215,11 @@
       <c r="L15" s="9"/>
     </row>
     <row r="16" spans="1:12" ht="15.4" customHeight="1">
-      <c r="A16" s="89"/>
-      <c r="B16" s="89"/>
-      <c r="C16" s="89"/>
-      <c r="D16" s="89"/>
-      <c r="E16" s="89"/>
+      <c r="A16" s="87"/>
+      <c r="B16" s="87"/>
+      <c r="C16" s="87"/>
+      <c r="D16" s="87"/>
+      <c r="E16" s="87"/>
       <c r="F16" s="46"/>
       <c r="G16" s="46"/>
       <c r="H16" s="46"/>
@@ -1227,15 +1227,15 @@
       <c r="L16" s="10"/>
     </row>
     <row r="17" spans="1:12" ht="17.350000000000001" customHeight="1">
-      <c r="A17" s="77" t="s">
+      <c r="A17" s="86" t="s">
         <v>67</v>
       </c>
-      <c r="B17" s="77"/>
-      <c r="C17" s="77" t="s">
+      <c r="B17" s="86"/>
+      <c r="C17" s="86" t="s">
         <v>9</v>
       </c>
-      <c r="D17" s="77"/>
-      <c r="E17" s="77"/>
+      <c r="D17" s="86"/>
+      <c r="E17" s="86"/>
       <c r="F17" s="6" t="s">
         <v>5</v>
       </c>
@@ -1245,15 +1245,15 @@
       <c r="L17" s="10"/>
     </row>
     <row r="18" spans="1:12" ht="18.850000000000001" customHeight="1">
-      <c r="A18" s="85" t="s">
+      <c r="A18" s="84" t="s">
         <v>53</v>
       </c>
-      <c r="B18" s="85"/>
-      <c r="C18" s="86" t="s">
+      <c r="B18" s="84"/>
+      <c r="C18" s="85" t="s">
         <v>63</v>
       </c>
-      <c r="D18" s="86"/>
-      <c r="E18" s="86"/>
+      <c r="D18" s="85"/>
+      <c r="E18" s="85"/>
       <c r="F18" s="6" t="s">
         <v>5</v>
       </c>
@@ -1263,13 +1263,13 @@
       <c r="L18" s="10"/>
     </row>
     <row r="19" spans="1:12" ht="17.350000000000001" customHeight="1">
-      <c r="A19" s="77" t="s">
+      <c r="A19" s="86" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="77"/>
-      <c r="C19" s="82"/>
-      <c r="D19" s="82"/>
-      <c r="E19" s="82"/>
+      <c r="B19" s="86"/>
+      <c r="C19" s="92"/>
+      <c r="D19" s="92"/>
+      <c r="E19" s="92"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
@@ -1277,13 +1277,13 @@
       <c r="L19" s="10"/>
     </row>
     <row r="20" spans="1:12" ht="18.850000000000001" customHeight="1">
-      <c r="A20" s="83" t="s">
+      <c r="A20" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="B20" s="83"/>
-      <c r="C20" s="84"/>
-      <c r="D20" s="84"/>
-      <c r="E20" s="84"/>
+      <c r="B20" s="93"/>
+      <c r="C20" s="94"/>
+      <c r="D20" s="94"/>
+      <c r="E20" s="94"/>
       <c r="F20" s="65" t="s">
         <v>5</v>
       </c>
@@ -1293,19 +1293,19 @@
       <c r="L20" s="10"/>
     </row>
     <row r="21" spans="1:12" ht="12" customHeight="1">
-      <c r="A21" s="77" t="s">
+      <c r="A21" s="86" t="s">
         <v>11</v>
       </c>
-      <c r="B21" s="77"/>
-      <c r="C21" s="77"/>
-      <c r="D21" s="77"/>
-      <c r="E21" s="77"/>
+      <c r="B21" s="86"/>
+      <c r="C21" s="86"/>
+      <c r="D21" s="86"/>
+      <c r="E21" s="86"/>
       <c r="F21" s="12"/>
       <c r="G21" s="12"/>
-      <c r="H21" s="78" t="s">
+      <c r="H21" s="88" t="s">
         <v>12</v>
       </c>
-      <c r="I21" s="78"/>
+      <c r="I21" s="88"/>
       <c r="L21" s="10"/>
     </row>
     <row r="22" spans="1:12" ht="19.899999999999999" customHeight="1">
@@ -1440,10 +1440,10 @@
       </c>
       <c r="D33" s="15"/>
       <c r="E33" s="43"/>
-      <c r="F33" s="79" t="s">
+      <c r="F33" s="89" t="s">
         <v>59</v>
       </c>
-      <c r="G33" s="79"/>
+      <c r="G33" s="89"/>
       <c r="H33" s="36" t="s">
         <v>56</v>
       </c>
@@ -1899,28 +1899,12 @@
       <c r="B69" s="58"/>
       <c r="C69" s="64"/>
       <c r="D69" s="25"/>
-      <c r="G69" s="80"/>
-      <c r="H69" s="81"/>
-      <c r="I69" s="81"/>
+      <c r="G69" s="90"/>
+      <c r="H69" s="91"/>
+      <c r="I69" s="91"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="A6:E6"/>
-    <mergeCell ref="A7:E7"/>
-    <mergeCell ref="A8:E8"/>
-    <mergeCell ref="A9:E11"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="A12:E12"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="A14:E16"/>
     <mergeCell ref="A21:E21"/>
     <mergeCell ref="H21:I21"/>
     <mergeCell ref="F33:G33"/>
@@ -1929,6 +1913,22 @@
     <mergeCell ref="C19:E19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="C20:E20"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="A12:E12"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="A14:E16"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="A8:E8"/>
+    <mergeCell ref="A9:E11"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="F4:H4"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.35433070866141736" right="0.35433070866141736" top="0.59055118110236227" bottom="0.19685039370078741" header="0" footer="0"/>

</xml_diff>

<commit_message>
bl catchZone input field added
</commit_message>
<xml_diff>
--- a/templates/BL.xlsx
+++ b/templates/BL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F095979-2E9E-4041-BF3B-AE541B1BE505}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBEDCC6E-B22C-4744-ADA4-96CEEE65A3DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="27076" windowHeight="16395" tabRatio="667" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-57697" yWindow="-277" windowWidth="28995" windowHeight="16394" tabRatio="667" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BL" sheetId="10" r:id="rId1"/>
@@ -669,59 +669,59 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1005,7 +1005,7 @@
   <dimension ref="A1:N69"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6" defaultRowHeight="10.15"/>
@@ -1033,58 +1033,58 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="12" customHeight="1">
-      <c r="A2" s="77" t="s">
+      <c r="A2" s="92" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="77"/>
-      <c r="C2" s="77"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="77"/>
+      <c r="B2" s="92"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="4"/>
     </row>
     <row r="3" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A3" s="78" t="s">
+      <c r="A3" s="87" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="78"/>
-      <c r="C3" s="78"/>
-      <c r="D3" s="78"/>
-      <c r="E3" s="78"/>
-      <c r="F3" s="79" t="s">
+      <c r="B3" s="87"/>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="93" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="79"/>
-      <c r="H3" s="79"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="93"/>
       <c r="I3" s="2" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="13.5" customHeight="1">
-      <c r="A4" s="80" t="s">
+      <c r="A4" s="88" t="s">
         <v>51</v>
       </c>
-      <c r="B4" s="80"/>
-      <c r="C4" s="80"/>
-      <c r="D4" s="80"/>
-      <c r="E4" s="80"/>
-      <c r="F4" s="81" t="s">
+      <c r="B4" s="88"/>
+      <c r="C4" s="88"/>
+      <c r="D4" s="88"/>
+      <c r="E4" s="88"/>
+      <c r="F4" s="94" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="81"/>
-      <c r="H4" s="81"/>
+      <c r="G4" s="94"/>
+      <c r="H4" s="94"/>
       <c r="I4" s="6"/>
     </row>
     <row r="5" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A5" s="80" t="s">
+      <c r="A5" s="88" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="80"/>
-      <c r="C5" s="80"/>
-      <c r="D5" s="80"/>
-      <c r="E5" s="80"/>
+      <c r="B5" s="88"/>
+      <c r="C5" s="88"/>
+      <c r="D5" s="88"/>
+      <c r="E5" s="88"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
       <c r="H5" s="7" t="s">
@@ -1093,82 +1093,82 @@
       <c r="I5" s="7"/>
     </row>
     <row r="6" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A6" s="82"/>
-      <c r="B6" s="82"/>
-      <c r="C6" s="82"/>
-      <c r="D6" s="82"/>
-      <c r="E6" s="82"/>
+      <c r="A6" s="90"/>
+      <c r="B6" s="90"/>
+      <c r="C6" s="90"/>
+      <c r="D6" s="90"/>
+      <c r="E6" s="90"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
     </row>
     <row r="7" spans="1:12" ht="12" customHeight="1">
-      <c r="A7" s="78" t="s">
+      <c r="A7" s="87" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="78"/>
-      <c r="C7" s="78"/>
-      <c r="D7" s="78"/>
-      <c r="E7" s="78"/>
+      <c r="B7" s="87"/>
+      <c r="C7" s="87"/>
+      <c r="D7" s="87"/>
+      <c r="E7" s="87"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
     </row>
     <row r="8" spans="1:12" ht="12" customHeight="1">
-      <c r="A8" s="83" t="s">
+      <c r="A8" s="91" t="s">
         <v>66</v>
       </c>
-      <c r="B8" s="83"/>
-      <c r="C8" s="83"/>
-      <c r="D8" s="83"/>
-      <c r="E8" s="83"/>
+      <c r="B8" s="91"/>
+      <c r="C8" s="91"/>
+      <c r="D8" s="91"/>
+      <c r="E8" s="91"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
     </row>
     <row r="9" spans="1:12" ht="15.4" customHeight="1">
-      <c r="A9" s="80" t="s">
+      <c r="A9" s="88" t="s">
         <v>65</v>
       </c>
-      <c r="B9" s="80"/>
-      <c r="C9" s="80"/>
-      <c r="D9" s="80"/>
-      <c r="E9" s="80"/>
+      <c r="B9" s="88"/>
+      <c r="C9" s="88"/>
+      <c r="D9" s="88"/>
+      <c r="E9" s="88"/>
       <c r="I9" s="6"/>
     </row>
     <row r="10" spans="1:12" ht="15.4" customHeight="1">
-      <c r="A10" s="80"/>
-      <c r="B10" s="80"/>
-      <c r="C10" s="80"/>
-      <c r="D10" s="80"/>
-      <c r="E10" s="80"/>
+      <c r="A10" s="88"/>
+      <c r="B10" s="88"/>
+      <c r="C10" s="88"/>
+      <c r="D10" s="88"/>
+      <c r="E10" s="88"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
     </row>
     <row r="11" spans="1:12" ht="15.4" customHeight="1">
-      <c r="A11" s="80"/>
-      <c r="B11" s="80"/>
-      <c r="C11" s="80"/>
-      <c r="D11" s="80"/>
-      <c r="E11" s="80"/>
+      <c r="A11" s="88"/>
+      <c r="B11" s="88"/>
+      <c r="C11" s="88"/>
+      <c r="D11" s="88"/>
+      <c r="E11" s="88"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
     </row>
     <row r="12" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A12" s="78" t="s">
+      <c r="A12" s="87" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="78"/>
-      <c r="C12" s="78"/>
-      <c r="D12" s="78"/>
-      <c r="E12" s="78"/>
+      <c r="B12" s="87"/>
+      <c r="C12" s="87"/>
+      <c r="D12" s="87"/>
+      <c r="E12" s="87"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
@@ -1188,24 +1188,24 @@
       <c r="I13" s="69"/>
     </row>
     <row r="14" spans="1:12" ht="15.4" customHeight="1">
-      <c r="A14" s="80" t="s">
+      <c r="A14" s="88" t="s">
         <v>68</v>
       </c>
-      <c r="B14" s="80"/>
-      <c r="C14" s="80"/>
-      <c r="D14" s="80"/>
-      <c r="E14" s="80"/>
+      <c r="B14" s="88"/>
+      <c r="C14" s="88"/>
+      <c r="D14" s="88"/>
+      <c r="E14" s="88"/>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
     </row>
     <row r="15" spans="1:12" ht="15.4" customHeight="1">
-      <c r="A15" s="80"/>
-      <c r="B15" s="80"/>
-      <c r="C15" s="80"/>
-      <c r="D15" s="80"/>
-      <c r="E15" s="80"/>
+      <c r="A15" s="88"/>
+      <c r="B15" s="88"/>
+      <c r="C15" s="88"/>
+      <c r="D15" s="88"/>
+      <c r="E15" s="88"/>
       <c r="F15" s="7"/>
       <c r="G15" s="7" t="s">
         <v>5</v>
@@ -1215,11 +1215,11 @@
       <c r="L15" s="9"/>
     </row>
     <row r="16" spans="1:12" ht="15.4" customHeight="1">
-      <c r="A16" s="87"/>
-      <c r="B16" s="87"/>
-      <c r="C16" s="87"/>
-      <c r="D16" s="87"/>
-      <c r="E16" s="87"/>
+      <c r="A16" s="89"/>
+      <c r="B16" s="89"/>
+      <c r="C16" s="89"/>
+      <c r="D16" s="89"/>
+      <c r="E16" s="89"/>
       <c r="F16" s="46"/>
       <c r="G16" s="46"/>
       <c r="H16" s="46"/>
@@ -1227,15 +1227,15 @@
       <c r="L16" s="10"/>
     </row>
     <row r="17" spans="1:12" ht="17.350000000000001" customHeight="1">
-      <c r="A17" s="86" t="s">
+      <c r="A17" s="77" t="s">
         <v>67</v>
       </c>
-      <c r="B17" s="86"/>
-      <c r="C17" s="86" t="s">
+      <c r="B17" s="77"/>
+      <c r="C17" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="D17" s="86"/>
-      <c r="E17" s="86"/>
+      <c r="D17" s="77"/>
+      <c r="E17" s="77"/>
       <c r="F17" s="6" t="s">
         <v>5</v>
       </c>
@@ -1245,15 +1245,15 @@
       <c r="L17" s="10"/>
     </row>
     <row r="18" spans="1:12" ht="18.850000000000001" customHeight="1">
-      <c r="A18" s="84" t="s">
+      <c r="A18" s="85" t="s">
         <v>53</v>
       </c>
-      <c r="B18" s="84"/>
-      <c r="C18" s="85" t="s">
+      <c r="B18" s="85"/>
+      <c r="C18" s="86" t="s">
         <v>63</v>
       </c>
-      <c r="D18" s="85"/>
-      <c r="E18" s="85"/>
+      <c r="D18" s="86"/>
+      <c r="E18" s="86"/>
       <c r="F18" s="6" t="s">
         <v>5</v>
       </c>
@@ -1263,13 +1263,13 @@
       <c r="L18" s="10"/>
     </row>
     <row r="19" spans="1:12" ht="17.350000000000001" customHeight="1">
-      <c r="A19" s="86" t="s">
+      <c r="A19" s="77" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="86"/>
-      <c r="C19" s="92"/>
-      <c r="D19" s="92"/>
-      <c r="E19" s="92"/>
+      <c r="B19" s="77"/>
+      <c r="C19" s="82"/>
+      <c r="D19" s="82"/>
+      <c r="E19" s="82"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
@@ -1277,13 +1277,13 @@
       <c r="L19" s="10"/>
     </row>
     <row r="20" spans="1:12" ht="18.850000000000001" customHeight="1">
-      <c r="A20" s="93" t="s">
+      <c r="A20" s="83" t="s">
         <v>54</v>
       </c>
-      <c r="B20" s="93"/>
-      <c r="C20" s="94"/>
-      <c r="D20" s="94"/>
-      <c r="E20" s="94"/>
+      <c r="B20" s="83"/>
+      <c r="C20" s="84"/>
+      <c r="D20" s="84"/>
+      <c r="E20" s="84"/>
       <c r="F20" s="65" t="s">
         <v>5</v>
       </c>
@@ -1293,19 +1293,19 @@
       <c r="L20" s="10"/>
     </row>
     <row r="21" spans="1:12" ht="12" customHeight="1">
-      <c r="A21" s="86" t="s">
+      <c r="A21" s="77" t="s">
         <v>11</v>
       </c>
-      <c r="B21" s="86"/>
-      <c r="C21" s="86"/>
-      <c r="D21" s="86"/>
-      <c r="E21" s="86"/>
+      <c r="B21" s="77"/>
+      <c r="C21" s="77"/>
+      <c r="D21" s="77"/>
+      <c r="E21" s="77"/>
       <c r="F21" s="12"/>
       <c r="G21" s="12"/>
-      <c r="H21" s="88" t="s">
+      <c r="H21" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="I21" s="88"/>
+      <c r="I21" s="78"/>
       <c r="L21" s="10"/>
     </row>
     <row r="22" spans="1:12" ht="19.899999999999999" customHeight="1">
@@ -1440,10 +1440,10 @@
       </c>
       <c r="D33" s="15"/>
       <c r="E33" s="43"/>
-      <c r="F33" s="89" t="s">
+      <c r="F33" s="79" t="s">
         <v>59</v>
       </c>
-      <c r="G33" s="89"/>
+      <c r="G33" s="79"/>
       <c r="H33" s="36" t="s">
         <v>56</v>
       </c>
@@ -1899,12 +1899,28 @@
       <c r="B69" s="58"/>
       <c r="C69" s="64"/>
       <c r="D69" s="25"/>
-      <c r="G69" s="90"/>
-      <c r="H69" s="91"/>
-      <c r="I69" s="91"/>
+      <c r="G69" s="80"/>
+      <c r="H69" s="81"/>
+      <c r="I69" s="81"/>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="A8:E8"/>
+    <mergeCell ref="A9:E11"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="A12:E12"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="A14:E16"/>
     <mergeCell ref="A21:E21"/>
     <mergeCell ref="H21:I21"/>
     <mergeCell ref="F33:G33"/>
@@ -1913,22 +1929,6 @@
     <mergeCell ref="C19:E19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="C20:E20"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="A12:E12"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="A14:E16"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="A6:E6"/>
-    <mergeCell ref="A7:E7"/>
-    <mergeCell ref="A8:E8"/>
-    <mergeCell ref="A9:E11"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="F4:H4"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.35433070866141736" right="0.35433070866141736" top="0.59055118110236227" bottom="0.19685039370078741" header="0" footer="0"/>

</xml_diff>

<commit_message>
bl tmp hidden rows fixed
</commit_message>
<xml_diff>
--- a/templates/BL.xlsx
+++ b/templates/BL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBEDCC6E-B22C-4744-ADA4-96CEEE65A3DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F415CCD4-794B-461E-966D-74CAFFADFDA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57697" yWindow="-277" windowWidth="28995" windowHeight="16394" tabRatio="667" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" tabRatio="667" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BL" sheetId="10" r:id="rId1"/>
@@ -669,9 +669,39 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -692,36 +722,6 @@
     </xf>
     <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1005,7 +1005,7 @@
   <dimension ref="A1:N69"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6" defaultRowHeight="10.15"/>
@@ -1033,58 +1033,58 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="12" customHeight="1">
-      <c r="A2" s="92" t="s">
+      <c r="A2" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="92"/>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="92"/>
+      <c r="B2" s="77"/>
+      <c r="C2" s="77"/>
+      <c r="D2" s="77"/>
+      <c r="E2" s="77"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="4"/>
     </row>
     <row r="3" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A3" s="87" t="s">
+      <c r="A3" s="78" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="87"/>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="93" t="s">
+      <c r="B3" s="78"/>
+      <c r="C3" s="78"/>
+      <c r="D3" s="78"/>
+      <c r="E3" s="78"/>
+      <c r="F3" s="79" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="93"/>
-      <c r="H3" s="93"/>
+      <c r="G3" s="79"/>
+      <c r="H3" s="79"/>
       <c r="I3" s="2" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="13.5" customHeight="1">
-      <c r="A4" s="88" t="s">
+      <c r="A4" s="80" t="s">
         <v>51</v>
       </c>
-      <c r="B4" s="88"/>
-      <c r="C4" s="88"/>
-      <c r="D4" s="88"/>
-      <c r="E4" s="88"/>
-      <c r="F4" s="94" t="s">
+      <c r="B4" s="80"/>
+      <c r="C4" s="80"/>
+      <c r="D4" s="80"/>
+      <c r="E4" s="80"/>
+      <c r="F4" s="81" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="94"/>
-      <c r="H4" s="94"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="81"/>
       <c r="I4" s="6"/>
     </row>
     <row r="5" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A5" s="88" t="s">
+      <c r="A5" s="80" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="88"/>
-      <c r="C5" s="88"/>
-      <c r="D5" s="88"/>
-      <c r="E5" s="88"/>
+      <c r="B5" s="80"/>
+      <c r="C5" s="80"/>
+      <c r="D5" s="80"/>
+      <c r="E5" s="80"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
       <c r="H5" s="7" t="s">
@@ -1093,82 +1093,82 @@
       <c r="I5" s="7"/>
     </row>
     <row r="6" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A6" s="90"/>
-      <c r="B6" s="90"/>
-      <c r="C6" s="90"/>
-      <c r="D6" s="90"/>
-      <c r="E6" s="90"/>
+      <c r="A6" s="82"/>
+      <c r="B6" s="82"/>
+      <c r="C6" s="82"/>
+      <c r="D6" s="82"/>
+      <c r="E6" s="82"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
     </row>
     <row r="7" spans="1:12" ht="12" customHeight="1">
-      <c r="A7" s="87" t="s">
+      <c r="A7" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="87"/>
-      <c r="C7" s="87"/>
-      <c r="D7" s="87"/>
-      <c r="E7" s="87"/>
+      <c r="B7" s="78"/>
+      <c r="C7" s="78"/>
+      <c r="D7" s="78"/>
+      <c r="E7" s="78"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
     </row>
     <row r="8" spans="1:12" ht="12" customHeight="1">
-      <c r="A8" s="91" t="s">
+      <c r="A8" s="83" t="s">
         <v>66</v>
       </c>
-      <c r="B8" s="91"/>
-      <c r="C8" s="91"/>
-      <c r="D8" s="91"/>
-      <c r="E8" s="91"/>
+      <c r="B8" s="83"/>
+      <c r="C8" s="83"/>
+      <c r="D8" s="83"/>
+      <c r="E8" s="83"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
     </row>
     <row r="9" spans="1:12" ht="15.4" customHeight="1">
-      <c r="A9" s="88" t="s">
+      <c r="A9" s="80" t="s">
         <v>65</v>
       </c>
-      <c r="B9" s="88"/>
-      <c r="C9" s="88"/>
-      <c r="D9" s="88"/>
-      <c r="E9" s="88"/>
+      <c r="B9" s="80"/>
+      <c r="C9" s="80"/>
+      <c r="D9" s="80"/>
+      <c r="E9" s="80"/>
       <c r="I9" s="6"/>
     </row>
     <row r="10" spans="1:12" ht="15.4" customHeight="1">
-      <c r="A10" s="88"/>
-      <c r="B10" s="88"/>
-      <c r="C10" s="88"/>
-      <c r="D10" s="88"/>
-      <c r="E10" s="88"/>
+      <c r="A10" s="80"/>
+      <c r="B10" s="80"/>
+      <c r="C10" s="80"/>
+      <c r="D10" s="80"/>
+      <c r="E10" s="80"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
     </row>
     <row r="11" spans="1:12" ht="15.4" customHeight="1">
-      <c r="A11" s="88"/>
-      <c r="B11" s="88"/>
-      <c r="C11" s="88"/>
-      <c r="D11" s="88"/>
-      <c r="E11" s="88"/>
+      <c r="A11" s="80"/>
+      <c r="B11" s="80"/>
+      <c r="C11" s="80"/>
+      <c r="D11" s="80"/>
+      <c r="E11" s="80"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
     </row>
     <row r="12" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A12" s="87" t="s">
+      <c r="A12" s="78" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="87"/>
-      <c r="C12" s="87"/>
-      <c r="D12" s="87"/>
-      <c r="E12" s="87"/>
+      <c r="B12" s="78"/>
+      <c r="C12" s="78"/>
+      <c r="D12" s="78"/>
+      <c r="E12" s="78"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
@@ -1188,24 +1188,24 @@
       <c r="I13" s="69"/>
     </row>
     <row r="14" spans="1:12" ht="15.4" customHeight="1">
-      <c r="A14" s="88" t="s">
+      <c r="A14" s="80" t="s">
         <v>68</v>
       </c>
-      <c r="B14" s="88"/>
-      <c r="C14" s="88"/>
-      <c r="D14" s="88"/>
-      <c r="E14" s="88"/>
+      <c r="B14" s="80"/>
+      <c r="C14" s="80"/>
+      <c r="D14" s="80"/>
+      <c r="E14" s="80"/>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
     </row>
     <row r="15" spans="1:12" ht="15.4" customHeight="1">
-      <c r="A15" s="88"/>
-      <c r="B15" s="88"/>
-      <c r="C15" s="88"/>
-      <c r="D15" s="88"/>
-      <c r="E15" s="88"/>
+      <c r="A15" s="80"/>
+      <c r="B15" s="80"/>
+      <c r="C15" s="80"/>
+      <c r="D15" s="80"/>
+      <c r="E15" s="80"/>
       <c r="F15" s="7"/>
       <c r="G15" s="7" t="s">
         <v>5</v>
@@ -1215,11 +1215,11 @@
       <c r="L15" s="9"/>
     </row>
     <row r="16" spans="1:12" ht="15.4" customHeight="1">
-      <c r="A16" s="89"/>
-      <c r="B16" s="89"/>
-      <c r="C16" s="89"/>
-      <c r="D16" s="89"/>
-      <c r="E16" s="89"/>
+      <c r="A16" s="87"/>
+      <c r="B16" s="87"/>
+      <c r="C16" s="87"/>
+      <c r="D16" s="87"/>
+      <c r="E16" s="87"/>
       <c r="F16" s="46"/>
       <c r="G16" s="46"/>
       <c r="H16" s="46"/>
@@ -1227,15 +1227,15 @@
       <c r="L16" s="10"/>
     </row>
     <row r="17" spans="1:12" ht="17.350000000000001" customHeight="1">
-      <c r="A17" s="77" t="s">
+      <c r="A17" s="86" t="s">
         <v>67</v>
       </c>
-      <c r="B17" s="77"/>
-      <c r="C17" s="77" t="s">
+      <c r="B17" s="86"/>
+      <c r="C17" s="86" t="s">
         <v>9</v>
       </c>
-      <c r="D17" s="77"/>
-      <c r="E17" s="77"/>
+      <c r="D17" s="86"/>
+      <c r="E17" s="86"/>
       <c r="F17" s="6" t="s">
         <v>5</v>
       </c>
@@ -1245,15 +1245,15 @@
       <c r="L17" s="10"/>
     </row>
     <row r="18" spans="1:12" ht="18.850000000000001" customHeight="1">
-      <c r="A18" s="85" t="s">
+      <c r="A18" s="84" t="s">
         <v>53</v>
       </c>
-      <c r="B18" s="85"/>
-      <c r="C18" s="86" t="s">
+      <c r="B18" s="84"/>
+      <c r="C18" s="85" t="s">
         <v>63</v>
       </c>
-      <c r="D18" s="86"/>
-      <c r="E18" s="86"/>
+      <c r="D18" s="85"/>
+      <c r="E18" s="85"/>
       <c r="F18" s="6" t="s">
         <v>5</v>
       </c>
@@ -1263,13 +1263,13 @@
       <c r="L18" s="10"/>
     </row>
     <row r="19" spans="1:12" ht="17.350000000000001" customHeight="1">
-      <c r="A19" s="77" t="s">
+      <c r="A19" s="86" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="77"/>
-      <c r="C19" s="82"/>
-      <c r="D19" s="82"/>
-      <c r="E19" s="82"/>
+      <c r="B19" s="86"/>
+      <c r="C19" s="92"/>
+      <c r="D19" s="92"/>
+      <c r="E19" s="92"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
@@ -1277,13 +1277,13 @@
       <c r="L19" s="10"/>
     </row>
     <row r="20" spans="1:12" ht="18.850000000000001" customHeight="1">
-      <c r="A20" s="83" t="s">
+      <c r="A20" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="B20" s="83"/>
-      <c r="C20" s="84"/>
-      <c r="D20" s="84"/>
-      <c r="E20" s="84"/>
+      <c r="B20" s="93"/>
+      <c r="C20" s="94"/>
+      <c r="D20" s="94"/>
+      <c r="E20" s="94"/>
       <c r="F20" s="65" t="s">
         <v>5</v>
       </c>
@@ -1293,19 +1293,19 @@
       <c r="L20" s="10"/>
     </row>
     <row r="21" spans="1:12" ht="12" customHeight="1">
-      <c r="A21" s="77" t="s">
+      <c r="A21" s="86" t="s">
         <v>11</v>
       </c>
-      <c r="B21" s="77"/>
-      <c r="C21" s="77"/>
-      <c r="D21" s="77"/>
-      <c r="E21" s="77"/>
+      <c r="B21" s="86"/>
+      <c r="C21" s="86"/>
+      <c r="D21" s="86"/>
+      <c r="E21" s="86"/>
       <c r="F21" s="12"/>
       <c r="G21" s="12"/>
-      <c r="H21" s="78" t="s">
+      <c r="H21" s="88" t="s">
         <v>12</v>
       </c>
-      <c r="I21" s="78"/>
+      <c r="I21" s="88"/>
       <c r="L21" s="10"/>
     </row>
     <row r="22" spans="1:12" ht="19.899999999999999" customHeight="1">
@@ -1320,7 +1320,7 @@
       <c r="I22" s="8"/>
       <c r="L22" s="10"/>
     </row>
-    <row r="23" spans="1:12" ht="11.65" customHeight="1">
+    <row r="23" spans="1:12" ht="12.85" customHeight="1">
       <c r="A23" s="40"/>
       <c r="B23" s="40"/>
       <c r="C23" s="40"/>
@@ -1333,7 +1333,7 @@
       </c>
       <c r="I23" s="40"/>
     </row>
-    <row r="24" spans="1:12" ht="11.65" customHeight="1">
+    <row r="24" spans="1:12" ht="12.85" customHeight="1">
       <c r="A24" s="41"/>
       <c r="B24" s="40"/>
       <c r="C24" s="40"/>
@@ -1348,7 +1348,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:12" s="16" customFormat="1" ht="12.75" customHeight="1">
+    <row r="25" spans="1:12" s="16" customFormat="1" ht="12.85" customHeight="1">
       <c r="A25" s="14"/>
       <c r="E25" s="15"/>
       <c r="F25" s="15"/>
@@ -1362,7 +1362,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:12" s="16" customFormat="1" ht="12.75" customHeight="1">
+    <row r="26" spans="1:12" s="16" customFormat="1" ht="12.85" customHeight="1">
       <c r="A26" s="14"/>
       <c r="E26" s="15"/>
       <c r="F26" s="15"/>
@@ -1370,7 +1370,7 @@
       <c r="H26" s="18"/>
       <c r="I26" s="18"/>
     </row>
-    <row r="27" spans="1:12" s="16" customFormat="1" ht="12.75" customHeight="1">
+    <row r="27" spans="1:12" s="16" customFormat="1" ht="12.85" customHeight="1">
       <c r="A27" s="71" t="s">
         <v>69</v>
       </c>
@@ -1388,7 +1388,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:12" s="16" customFormat="1" ht="12.75" customHeight="1">
+    <row r="28" spans="1:12" s="16" customFormat="1" ht="12.85" customHeight="1">
       <c r="A28" s="14"/>
       <c r="E28" s="15"/>
       <c r="F28" s="15"/>
@@ -1396,7 +1396,7 @@
       <c r="H28" s="36"/>
       <c r="I28" s="36"/>
     </row>
-    <row r="29" spans="1:12" s="16" customFormat="1" ht="12.75" hidden="1" customHeight="1">
+    <row r="29" spans="1:12" s="16" customFormat="1" ht="12.85" customHeight="1">
       <c r="A29" s="14"/>
       <c r="E29" s="15"/>
       <c r="F29" s="15"/>
@@ -1404,7 +1404,7 @@
       <c r="H29" s="36"/>
       <c r="I29" s="36"/>
     </row>
-    <row r="30" spans="1:12" s="16" customFormat="1" ht="12.75" hidden="1" customHeight="1">
+    <row r="30" spans="1:12" s="16" customFormat="1" ht="12.85" customHeight="1">
       <c r="A30" s="14"/>
       <c r="E30" s="15"/>
       <c r="F30" s="15"/>
@@ -1412,7 +1412,7 @@
       <c r="H30" s="36"/>
       <c r="I30" s="36"/>
     </row>
-    <row r="31" spans="1:12" ht="11.65" customHeight="1">
+    <row r="31" spans="1:12" ht="12.85" customHeight="1">
       <c r="A31" s="42"/>
       <c r="B31" s="40"/>
       <c r="C31" s="40"/>
@@ -1423,7 +1423,7 @@
       <c r="H31" s="36"/>
       <c r="I31" s="36"/>
     </row>
-    <row r="32" spans="1:12" ht="11.65" customHeight="1">
+    <row r="32" spans="1:12" ht="12.85" customHeight="1">
       <c r="A32" s="42"/>
       <c r="B32" s="40"/>
       <c r="C32" s="40"/>
@@ -1434,16 +1434,16 @@
       <c r="H32" s="36"/>
       <c r="I32" s="36"/>
     </row>
-    <row r="33" spans="1:14" ht="11.65" customHeight="1">
+    <row r="33" spans="1:14" ht="12.85" customHeight="1">
       <c r="B33" s="40" t="s">
         <v>60</v>
       </c>
       <c r="D33" s="15"/>
       <c r="E33" s="43"/>
-      <c r="F33" s="79" t="s">
+      <c r="F33" s="89" t="s">
         <v>59</v>
       </c>
-      <c r="G33" s="79"/>
+      <c r="G33" s="89"/>
       <c r="H33" s="36" t="s">
         <v>56</v>
       </c>
@@ -1457,7 +1457,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="11.65" customHeight="1">
+    <row r="34" spans="1:14" ht="12.85" customHeight="1">
       <c r="A34" s="19"/>
       <c r="B34" s="8"/>
       <c r="C34" s="19"/>
@@ -1468,7 +1468,7 @@
       <c r="H34" s="20"/>
       <c r="I34" s="20"/>
     </row>
-    <row r="35" spans="1:14" ht="11.65" customHeight="1">
+    <row r="35" spans="1:14" ht="12.85" customHeight="1">
       <c r="A35" s="19"/>
       <c r="B35" s="8"/>
       <c r="C35" s="19"/>
@@ -1479,7 +1479,7 @@
       <c r="H35" s="20"/>
       <c r="I35" s="20"/>
     </row>
-    <row r="36" spans="1:14" ht="11.65" customHeight="1">
+    <row r="36" spans="1:14" ht="12.85" customHeight="1">
       <c r="A36" s="19"/>
       <c r="B36" s="8"/>
       <c r="C36" s="8"/>
@@ -1490,7 +1490,7 @@
       <c r="H36" s="8"/>
       <c r="I36" s="8"/>
     </row>
-    <row r="37" spans="1:14" ht="11.65" customHeight="1">
+    <row r="37" spans="1:14" ht="12.85" customHeight="1">
       <c r="A37" s="1"/>
       <c r="B37" s="8" t="s">
         <v>17</v>
@@ -1503,7 +1503,7 @@
       <c r="H37" s="8"/>
       <c r="I37" s="8"/>
     </row>
-    <row r="38" spans="1:14" ht="11.65" customHeight="1">
+    <row r="38" spans="1:14" ht="12.85" customHeight="1">
       <c r="B38" s="8" t="s">
         <v>18</v>
       </c>
@@ -1515,7 +1515,7 @@
       <c r="H38" s="8"/>
       <c r="I38" s="8"/>
     </row>
-    <row r="39" spans="1:14" ht="11.65" customHeight="1">
+    <row r="39" spans="1:14" ht="12.85" customHeight="1">
       <c r="A39" s="8"/>
       <c r="B39" s="66"/>
       <c r="C39" s="66"/>
@@ -1526,7 +1526,7 @@
       <c r="H39" s="66"/>
       <c r="I39" s="66"/>
     </row>
-    <row r="40" spans="1:14" ht="11.65" customHeight="1">
+    <row r="40" spans="1:14" ht="12.85" customHeight="1">
       <c r="A40" s="8"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -1537,7 +1537,7 @@
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="1:14" ht="11.65" customHeight="1">
+    <row r="41" spans="1:14" ht="12.85" customHeight="1">
       <c r="A41" s="6"/>
       <c r="B41" s="37" t="s">
         <v>19</v>
@@ -1554,7 +1554,7 @@
       <c r="H41" s="6"/>
       <c r="I41" s="6"/>
     </row>
-    <row r="42" spans="1:14" ht="12" customHeight="1">
+    <row r="42" spans="1:14" ht="12.85" customHeight="1">
       <c r="A42" s="6"/>
       <c r="B42" s="37" t="s">
         <v>22</v>
@@ -1899,28 +1899,12 @@
       <c r="B69" s="58"/>
       <c r="C69" s="64"/>
       <c r="D69" s="25"/>
-      <c r="G69" s="80"/>
-      <c r="H69" s="81"/>
-      <c r="I69" s="81"/>
+      <c r="G69" s="90"/>
+      <c r="H69" s="91"/>
+      <c r="I69" s="91"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="A6:E6"/>
-    <mergeCell ref="A7:E7"/>
-    <mergeCell ref="A8:E8"/>
-    <mergeCell ref="A9:E11"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="A12:E12"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="A14:E16"/>
     <mergeCell ref="A21:E21"/>
     <mergeCell ref="H21:I21"/>
     <mergeCell ref="F33:G33"/>
@@ -1929,6 +1913,22 @@
     <mergeCell ref="C19:E19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="C20:E20"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="A12:E12"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="A14:E16"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="A8:E8"/>
+    <mergeCell ref="A9:E11"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="F4:H4"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.35433070866141736" right="0.35433070866141736" top="0.59055118110236227" bottom="0.19685039370078741" header="0" footer="0"/>

</xml_diff>